<commit_message>
v0.5. ahora tiene textbox para rellenar el significado
</commit_message>
<xml_diff>
--- a/excel/verbosIrregulares.xlsx
+++ b/excel/verbosIrregulares.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapho\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapho\Documents\GIT\VerbosIrregulares\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{92D879AA-6185-4101-91A8-86DD9EA5F3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0B805E-F089-4D62-87B7-01C2461C68C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LIMPIO" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="214">
   <si>
     <t>INFINITIVE</t>
   </si>
@@ -418,9 +418,6 @@
   </si>
   <si>
     <t>ekarri</t>
-  </si>
-  <si>
-    <t>biuilt</t>
   </si>
   <si>
     <t>built</t>
@@ -690,7 +687,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -775,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -785,8 +782,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1026,26 +1022,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D93" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:D93"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:D93" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:D93" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="INFINITIVE" dataDxfId="8"/>
-    <tableColumn id="2" name="SIMPLE PAST" dataDxfId="7"/>
-    <tableColumn id="3" name="PAST PARTICIPLE" dataDxfId="6"/>
-    <tableColumn id="4" name="MEANING" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INFINITIVE" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SIMPLE PAST" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PAST PARTICIPLE" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MEANING" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A1:D48" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla13" displayName="Tabla13" ref="A1:D48" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D48" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="INFINITIVE" dataDxfId="3"/>
-    <tableColumn id="2" name="SIMPLE PAST" dataDxfId="2"/>
-    <tableColumn id="3" name="PAST PARTICIPLE" dataDxfId="1"/>
-    <tableColumn id="4" name="MEANING" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="INFINITIVE" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="SIMPLE PAST" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="PAST PARTICIPLE" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="MEANING" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1367,7 +1363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1879,11 +1875,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1926,7 +1922,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>98</v>
@@ -2027,10 +2023,10 @@
         <v>126</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -2038,13 +2034,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -2052,13 +2048,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2066,13 +2062,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -2080,13 +2076,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -2094,13 +2090,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2108,13 +2104,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>106</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2128,7 +2124,7 @@
         <v>107</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2142,7 +2138,7 @@
         <v>102</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2150,13 +2146,13 @@
         <v>21</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2164,13 +2160,13 @@
         <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2184,7 +2180,7 @@
         <v>118</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2192,13 +2188,13 @@
         <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2206,13 +2202,13 @@
         <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2220,13 +2216,13 @@
         <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>119</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2234,13 +2230,13 @@
         <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2248,13 +2244,13 @@
         <v>28</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>100</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2262,13 +2258,13 @@
         <v>29</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2276,13 +2272,13 @@
         <v>30</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2290,13 +2286,13 @@
         <v>31</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2304,13 +2300,13 @@
         <v>32</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2318,13 +2314,13 @@
         <v>33</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2332,13 +2328,13 @@
         <v>34</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -2346,13 +2342,13 @@
         <v>35</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -2360,13 +2356,13 @@
         <v>36</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -2374,13 +2370,13 @@
         <v>37</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -2388,13 +2384,13 @@
         <v>38</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -2402,13 +2398,13 @@
         <v>39</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -2416,13 +2412,13 @@
         <v>40</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -2430,13 +2426,13 @@
         <v>41</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -2444,13 +2440,13 @@
         <v>42</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -2458,13 +2454,13 @@
         <v>43</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -2472,13 +2468,13 @@
         <v>44</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -2486,13 +2482,13 @@
         <v>45</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -2500,13 +2496,13 @@
         <v>46</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -2514,13 +2510,13 @@
         <v>47</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -2528,13 +2524,13 @@
         <v>48</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -2542,298 +2538,163 @@
         <v>49</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="11" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="12" t="s">
+      <c r="C48" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="D48" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="C48" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="9"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="9"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="9"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="9"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="9"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="9"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="9"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="9"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="9"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="9"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="9"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="9"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="9"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="9"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="9"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="9"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="9"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="9"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="9"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="9"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="9"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="9"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="9"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="9"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="9"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="9"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="9"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="9"/>
-      <c r="B81" s="10"/>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="9"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="9"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="9"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="9"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="9"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="9"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="9"/>
-      <c r="B88" s="10"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="9"/>
-      <c r="B89" s="10"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="9"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="9"/>
-      <c r="B91" s="10"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="9"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="9"/>
-      <c r="B93" s="10"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
V1.0.0: proyecto terminado a falta de agrega el readme y editar el excel con la lista completa de verbos.
</commit_message>
<xml_diff>
--- a/excel/verbosIrregulares.xlsx
+++ b/excel/verbosIrregulares.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapho\Documents\GIT\VerbosIrregulares\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0B805E-F089-4D62-87B7-01C2461C68C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C8BBD6-66FA-4CB1-9725-9ADC59EF201F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1035,8 +1035,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla13" displayName="Tabla13" ref="A1:D48" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D48" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla13" displayName="Tabla13" ref="A1:D2" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="INFINITIVE" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="SIMPLE PAST" dataDxfId="2"/>
@@ -1878,8 +1878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
V1.1.0 corrección de errores.
</commit_message>
<xml_diff>
--- a/excel/verbosIrregulares.xlsx
+++ b/excel/verbosIrregulares.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapho\Documents\GIT\VerbosIrregulares\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C8BBD6-66FA-4CB1-9725-9ADC59EF201F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36ED345C-72D7-44C8-BC10-F3308BADA75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LIMPIO" sheetId="1" r:id="rId1"/>
-    <sheet name="COMPLETO" sheetId="2" r:id="rId2"/>
+    <sheet name="COMPLETO" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">LIMPIO!$1:$1</definedName>
@@ -772,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -782,123 +782,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1022,26 +910,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:D93" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:D93" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:D93" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INFINITIVE" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SIMPLE PAST" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PAST PARTICIPLE" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MEANING" dataDxfId="5"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla13" displayName="Tabla13" ref="A1:D2" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="INFINITIVE" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="SIMPLE PAST" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="PAST PARTICIPLE" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="MEANING" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INFINITIVE" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SIMPLE PAST" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PAST PARTICIPLE" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MEANING" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1371,7 +1246,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D93"/>
+      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1875,831 +1750,694 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671B5603-3844-40ED-BA4F-03BEA94A32A6}">
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="28.21875" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>213</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>117</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>126</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>126</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>128</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>136</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" t="s">
         <v>139</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>141</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>145</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
         <v>145</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>148</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>116</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>118</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
         <v>129</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>152</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>153</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>155</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>157</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>159</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>161</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
         <v>161</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>163</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
         <v>163</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
         <v>165</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" t="s">
         <v>165</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" t="s">
         <v>167</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" t="s">
         <v>167</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>169</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" t="s">
         <v>170</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" t="s">
         <v>172</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" t="s">
         <v>173</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" t="s">
         <v>175</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" t="s">
         <v>176</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" t="s">
         <v>178</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" t="s">
         <v>179</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" t="s">
         <v>183</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" t="s">
         <v>184</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" t="s">
         <v>186</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" t="s">
         <v>186</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" t="s">
         <v>188</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" t="s">
         <v>188</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" t="s">
         <v>190</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" t="s">
         <v>180</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" t="s">
         <v>192</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" t="s">
         <v>193</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" t="s">
         <v>195</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" t="s">
         <v>181</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" t="s">
         <v>197</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" t="s">
         <v>197</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" t="s">
         <v>199</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" t="s">
         <v>199</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" t="s">
         <v>201</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" t="s">
         <v>201</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" t="s">
         <v>203</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" t="s">
         <v>205</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" t="s">
         <v>204</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" t="s">
         <v>204</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" t="s">
         <v>209</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" t="s">
         <v>209</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" t="s">
         <v>207</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" t="s">
         <v>207</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
+      <c r="A48" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" t="s">
         <v>211</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" t="s">
         <v>211</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="D48" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="9"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="9"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="9"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="9"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="9"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="9"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="9"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="9"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="9"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="9"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="9"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="9"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="9"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="9"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="9"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="9"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="9"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="9"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="9"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="9"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="9"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="9"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="9"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="9"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="9"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="9"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="9"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="9"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="9"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="9"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="9"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="9"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="9"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="9"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="9"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="9"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="9"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="9"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="9"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="9"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="9"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="9"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="9"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>